<commit_message>
complete catchtrial question demo
</commit_message>
<xml_diff>
--- a/stim_table_initial.xlsx
+++ b/stim_table_initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8FC33BAC-4005-4799-805A-89FD9D18F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B73DE58D-7CF6-498F-A755-1FA1905C199D}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{8FC33BAC-4005-4799-805A-89FD9D18F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5D83E17-045F-4A03-8E0C-4E6B0FDA7B2D}"/>
   <bookViews>
-    <workbookView xWindow="-31935" yWindow="1170" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27855" yWindow="1800" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -228,10 +228,10 @@
     <t>blockNumber</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>catchtrialObj</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -304,6 +304,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,7 +576,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +614,7 @@
         <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -636,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -662,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -688,7 +692,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -714,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -740,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -766,7 +770,7 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -792,7 +796,7 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -818,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -844,7 +848,7 @@
         <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -870,7 +874,7 @@
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -896,7 +900,7 @@
         <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -922,7 +926,7 @@
         <v>31</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,7 +952,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,7 +978,7 @@
         <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,7 +1004,7 @@
         <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,7 +1030,7 @@
         <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1052,7 +1056,7 @@
         <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,7 +1082,7 @@
         <v>42</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1104,7 +1108,7 @@
         <v>43</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1130,7 +1134,7 @@
         <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1156,7 +1160,7 @@
         <v>50</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1182,7 +1186,7 @@
         <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1208,7 +1212,7 @@
         <v>52</v>
       </c>
       <c r="H24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1222,7 +1226,7 @@
         <v>100</v>
       </c>
       <c r="H25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create and add stimuli video to experiment. modify randomization script
</commit_message>
<xml_diff>
--- a/stim_table_initial.xlsx
+++ b/stim_table_initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{8FC33BAC-4005-4799-805A-89FD9D18F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5D83E17-045F-4A03-8E0C-4E6B0FDA7B2D}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{8FC33BAC-4005-4799-805A-89FD9D18F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28316CB4-96A0-48D1-A2C3-FB92244AFCCC}"/>
   <bookViews>
-    <workbookView xWindow="-27855" yWindow="1800" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36450" yWindow="-1575" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="79">
   <si>
     <t>stimDir</t>
   </si>
@@ -159,36 +159,6 @@
     <t>./stimuli/control_2.mp4</t>
   </si>
   <si>
-    <t>./stimuli/human_left_0.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_left_1.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_left_2.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_left_3.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_left_4.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_right_0.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_right_1.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_right_2.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_right_3.mp4</t>
-  </si>
-  <si>
-    <t>./stimuli/human_right_4.mp4</t>
-  </si>
-  <si>
     <t>./stimuli/robot_left_0.mp4</t>
   </si>
   <si>
@@ -232,6 +202,66 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_0_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_1_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_2_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_3_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_4_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_0_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_1_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_2_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_3_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_4_m.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_0_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_1_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_2_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_3_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_left_4_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_0_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_1_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_2_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_3_f.mp4</t>
+  </si>
+  <si>
+    <t>./stimuli/human_right_4_f.mp4</t>
   </si>
 </sst>
 </file>
@@ -282,7 +312,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -573,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +633,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
@@ -611,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -634,13 +674,13 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -660,13 +700,13 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -686,13 +726,13 @@
         <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -712,13 +752,13 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="G5">
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -738,13 +778,13 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G6">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -764,13 +804,13 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -790,13 +830,13 @@
         <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G8">
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -816,13 +856,13 @@
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G9">
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -842,13 +882,13 @@
         <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G10">
         <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,13 +908,13 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="G11">
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -882,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -894,13 +934,13 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -908,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -920,13 +960,13 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G13">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,10 +974,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -946,13 +986,13 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G14">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -960,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
@@ -972,13 +1012,13 @@
         <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="G15">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -986,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1">
         <v>4</v>
@@ -998,13 +1038,13 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="G16">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -1024,13 +1064,13 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1038,10 +1078,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -1050,13 +1090,13 @@
         <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G18">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1064,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -1076,13 +1116,13 @@
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="G19">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
@@ -1102,13 +1142,13 @@
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="G20">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1116,10 +1156,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
@@ -1128,13 +1168,13 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="G21">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1142,25 +1182,25 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1168,25 +1208,25 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G23">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1194,25 +1234,25 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G24">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1220,19 +1260,282 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
       </c>
       <c r="G25">
+        <v>33</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26">
+        <v>34</v>
+      </c>
+      <c r="H26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29">
+        <v>42</v>
+      </c>
+      <c r="H29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30">
+        <v>43</v>
+      </c>
+      <c r="H30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31">
+        <v>44</v>
+      </c>
+      <c r="H31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33">
+        <v>51</v>
+      </c>
+      <c r="H33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34">
+        <v>52</v>
+      </c>
+      <c r="H34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35">
         <v>100</v>
       </c>
-      <c r="H25" t="s">
-        <v>68</v>
+      <c r="H35" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>